<commit_message>
PTEN is now no longer an HR gene
</commit_message>
<xml_diff>
--- a/data/gene_selection/gene_list.xlsx
+++ b/data/gene_selection/gene_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lnguyen/hpc/cog_bioinf/cuppen/project_data/Luan_projects/CHORD/scripts_main/hmfGeneAnnotation/data/gene_selection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCDE9444-208A-914E-A52C-D9E12F8ABF86}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{996C427E-1439-5A43-BE83-3AC08E7B499F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="50340" yWindow="-6220" windowWidth="28360" windowHeight="21940" xr2:uid="{6BA42C94-802D-3F46-A81F-ACDA302C3A2E}"/>
+    <workbookView xWindow="45520" yWindow="-6280" windowWidth="28360" windowHeight="21940" xr2:uid="{6BA42C94-802D-3F46-A81F-ACDA302C3A2E}"/>
   </bookViews>
   <sheets>
     <sheet name="selected_genes" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,12 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -3120,8 +3126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{051348A4-375E-3245-A04C-EF55E2C9D34B}">
   <dimension ref="A1:G66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4243,7 +4249,7 @@
         <v>66</v>
       </c>
       <c r="F47" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G47" t="s">
         <v>70</v>

</xml_diff>